<commit_message>
Query file is updated
</commit_message>
<xml_diff>
--- a/QueryLogs.xlsx
+++ b/QueryLogs.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="23">
   <si>
     <t>S.No.</t>
   </si>
@@ -42,9 +42,6 @@
     <t>Reported to</t>
   </si>
   <si>
-    <t>Date</t>
-  </si>
-  <si>
     <t>Status</t>
   </si>
   <si>
@@ -66,9 +63,6 @@
     <t>What should be length of "Email" min and max</t>
   </si>
   <si>
-    <t>My understanding is that we can take 12 max size for phone</t>
-  </si>
-  <si>
     <t>25-06-2021</t>
   </si>
   <si>
@@ -81,7 +75,16 @@
     <t>If the record is more than 3, The what should be do</t>
   </si>
   <si>
-    <t>Understanding</t>
+    <t>Reported By</t>
+  </si>
+  <si>
+    <t>Reported Date</t>
+  </si>
+  <si>
+    <t>Respnce Date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I think, We should implement pagination </t>
   </si>
 </sst>
 </file>
@@ -97,12 +100,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -117,8 +126,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -413,60 +423,62 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K11"/>
+  <dimension ref="A1:L11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="12.85546875" customWidth="1"/>
     <col min="3" max="4" width="12.140625" customWidth="1"/>
-    <col min="5" max="5" width="53.5703125" customWidth="1"/>
-    <col min="6" max="6" width="49.28515625" customWidth="1"/>
-    <col min="7" max="7" width="19" customWidth="1"/>
-    <col min="8" max="8" width="17.85546875" customWidth="1"/>
-    <col min="9" max="9" width="11.85546875" customWidth="1"/>
-    <col min="10" max="10" width="10.5703125" customWidth="1"/>
+    <col min="5" max="5" width="49.28515625" customWidth="1"/>
+    <col min="6" max="6" width="35.85546875" customWidth="1"/>
+    <col min="7" max="9" width="17.85546875" customWidth="1"/>
+    <col min="10" max="10" width="11.85546875" customWidth="1"/>
+    <col min="11" max="11" width="12.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
-      <c r="A1" t="s">
+    <row r="1" spans="1:12">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="F1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" t="s">
-        <v>7</v>
-      </c>
-      <c r="J1" t="s">
+      <c r="L1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11">
+    </row>
+    <row r="2" spans="1:12">
       <c r="A2">
         <v>1</v>
       </c>
@@ -477,22 +489,22 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="D2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" t="s">
         <v>10</v>
       </c>
-      <c r="F2" t="s">
+      <c r="J2" t="s">
         <v>11</v>
       </c>
-      <c r="I2" t="s">
+      <c r="K2" t="s">
         <v>12</v>
       </c>
-      <c r="J2" t="s">
+      <c r="L2" t="s">
         <v>13</v>
       </c>
-      <c r="K2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11">
+    </row>
+    <row r="3" spans="1:12">
       <c r="A3">
         <v>2</v>
       </c>
@@ -502,20 +514,20 @@
       <c r="C3">
         <v>1.2</v>
       </c>
-      <c r="F3" t="s">
+      <c r="E3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J3" t="s">
+        <v>11</v>
+      </c>
+      <c r="K3" t="s">
         <v>15</v>
       </c>
-      <c r="I3" t="s">
-        <v>12</v>
-      </c>
-      <c r="J3" t="s">
-        <v>17</v>
-      </c>
-      <c r="K3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11">
+      <c r="L3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12">
       <c r="A4">
         <v>3</v>
       </c>
@@ -525,62 +537,62 @@
       <c r="C4">
         <v>1.3</v>
       </c>
-      <c r="E4" t="s">
+      <c r="J4" t="s">
+        <v>11</v>
+      </c>
+      <c r="K4" t="s">
         <v>16</v>
       </c>
-      <c r="I4" t="s">
-        <v>12</v>
-      </c>
-      <c r="J4" t="s">
-        <v>18</v>
-      </c>
-      <c r="K4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11">
+      <c r="L4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12">
       <c r="A5">
         <v>4</v>
       </c>
+      <c r="E5" t="s">
+        <v>18</v>
+      </c>
       <c r="F5" t="s">
-        <v>20</v>
-      </c>
-      <c r="I5" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="J5" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="K5" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11">
+        <v>17</v>
+      </c>
+      <c r="L5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12">
       <c r="A6">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:11">
+    <row r="7" spans="1:12">
       <c r="A7">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:11">
+    <row r="8" spans="1:12">
       <c r="A8">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:11">
+    <row r="9" spans="1:12">
       <c r="A9">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:11">
+    <row r="10" spans="1:12">
       <c r="A10">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:11">
+    <row r="11" spans="1:12">
       <c r="A11">
         <v>10</v>
       </c>

</xml_diff>